<commit_message>
Cover Test scenarios for Homepage Cartpage and Checkoutpage
</commit_message>
<xml_diff>
--- a/SauceLabs_TestCases.xlsx
+++ b/SauceLabs_TestCases.xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aravindkumar\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aravindkumar\Documents\SDET_Playwright\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284FE1F2-1F17-4001-87F1-176B6710A0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A2F7E6-561E-45AF-BB02-F79C053E9EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FB84D915-DA4F-4F24-AA98-55DFE3D8FD48}"/>
+    <workbookView xWindow="3564" yWindow="1020" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{FB84D915-DA4F-4F24-AA98-55DFE3D8FD48}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Flow" sheetId="1" r:id="rId1"/>
     <sheet name="Home Page" sheetId="2" r:id="rId2"/>
-    <sheet name="Checkout Page " sheetId="5" r:id="rId3"/>
-    <sheet name="Cart Page" sheetId="3" r:id="rId4"/>
-    <sheet name="PDP Page" sheetId="4" r:id="rId5"/>
+    <sheet name="Cart Page" sheetId="3" r:id="rId3"/>
+    <sheet name="Checkout Page " sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="90">
   <si>
     <t>Test case ID</t>
   </si>
@@ -166,6 +165,212 @@
   </si>
   <si>
     <t>Regression</t>
+  </si>
+  <si>
+    <t>TC101</t>
+  </si>
+  <si>
+    <t>Verify that whether user lands on Home page after login</t>
+  </si>
+  <si>
+    <t>TC102</t>
+  </si>
+  <si>
+    <t>Verify that whether user able to add product to the cart from home page</t>
+  </si>
+  <si>
+    <t>User is on Home page</t>
+  </si>
+  <si>
+    <t>1. User clicks on Add to cart button on any product from home page
+2. Verify the Add to cart button</t>
+  </si>
+  <si>
+    <t>1. Product gets added to the cart
+2. Add to cart button changes to Remove button</t>
+  </si>
+  <si>
+    <t>TC103</t>
+  </si>
+  <si>
+    <t>Verify the user able to remove the product from the cart</t>
+  </si>
+  <si>
+    <t>User is on Home page
+Product is added to the cart</t>
+  </si>
+  <si>
+    <t>1. User is on Home page
+2. Click the Remove button in the product
+3. Verify the Remove button</t>
+  </si>
+  <si>
+    <t>2. Product gets removed from cart
+3. Remove button changes back to Add to cart button</t>
+  </si>
+  <si>
+    <t>TC104</t>
+  </si>
+  <si>
+    <t>Footer - Verify the footer in the Home page</t>
+  </si>
+  <si>
+    <t>1. Scroll down to the footer 
+2. Verify the copyright year, social media links like Facebook, Twitter and LinkedIn</t>
+  </si>
+  <si>
+    <t>2. Current year should be displayed for copyright and user should able to navigate to the respective social media links.</t>
+  </si>
+  <si>
+    <t>TC105</t>
+  </si>
+  <si>
+    <t>Logout - Verify whether user is able to logout from Home page</t>
+  </si>
+  <si>
+    <t>1. Click on left side menu bar icon
+2. Click on Log out button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. User should be lands on login page </t>
+  </si>
+  <si>
+    <t>TC201</t>
+  </si>
+  <si>
+    <t>Verify the cart page after user added product to the cart</t>
+  </si>
+  <si>
+    <t>Product is added to the cart</t>
+  </si>
+  <si>
+    <t>1. Click on cart icon from the top
+2. Verify the cart page details</t>
+  </si>
+  <si>
+    <t>1. Cart page will be displayed
+2. Added product should be displayed with quantity, price and Remove button. Also, Continue Shopping and Checkout button should be displayed</t>
+  </si>
+  <si>
+    <t>TC202</t>
+  </si>
+  <si>
+    <t>Verify the page after user clicks on Checkout button from cart page</t>
+  </si>
+  <si>
+    <t>1. Cart page will be displayed
+2. Added product should be displayed with quantity, price and Remove button. 
+3. Checkout: Your information page should be displayed</t>
+  </si>
+  <si>
+    <t>TC203</t>
+  </si>
+  <si>
+    <t>Verify the page after user clicks on Remove button from cart page</t>
+  </si>
+  <si>
+    <t>1. Cart page will be displayed
+2. Product should be removed from cart page and empty cart will be displayed</t>
+  </si>
+  <si>
+    <t>TC204</t>
+  </si>
+  <si>
+    <t>Verify the page after user clicks on Continue Shopping button from cart page</t>
+  </si>
+  <si>
+    <t>1. Click on cart icon from the home page
+2. Click on Remove button</t>
+  </si>
+  <si>
+    <t>1. Click on cart icon from the home page
+2. Click on Continue Shopping button</t>
+  </si>
+  <si>
+    <t>1. Cart page will be displayed
+2. It will nagivate to the Home page</t>
+  </si>
+  <si>
+    <t>1. Click on cart icon from the home page
+2. Verify the product details
+3. Click on Checkout button</t>
+  </si>
+  <si>
+    <t>TC301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify the checkout step one page </t>
+  </si>
+  <si>
+    <t>Registered user is signed in
+Product is added to the user</t>
+  </si>
+  <si>
+    <t>1. Click on Cart icon from Home page
+2. Click on Checkout button
+3. Enters the user information
+4. Click the Continue button</t>
+  </si>
+  <si>
+    <t>TC302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify the checkout step two page </t>
+  </si>
+  <si>
+    <t>1. Click on Cart icon from Home page
+2. Click on Checkout button
+3. Enters the user information
+4. Click the Continue button
+5. Verify the product details, payment information, Shipping information, total price</t>
+  </si>
+  <si>
+    <t>1. Cart page will be displayed
+2. Checkout: Your information page will be displayed
+3. Fill the First Name, Last Name, Zip/Postal Code fields
+4. Checkout: Overview will be displayed
+5. Product details, total price with tax, payment and shipping information should be displayed correctly.</t>
+  </si>
+  <si>
+    <t>TC303</t>
+  </si>
+  <si>
+    <t>Verify that user should able to place an order successfully</t>
+  </si>
+  <si>
+    <t>Registered user is signed in
+Product is added to the user
+User is on checkout page</t>
+  </si>
+  <si>
+    <t>1. Verify the product information
+2. Click on Finish button</t>
+  </si>
+  <si>
+    <t>1.  Product details, total price with tax, payment and shipping information should be displayed correctly.
+2. Order should be placed successfully and "Thank you for your order!" message should be displayed with Back Home button</t>
+  </si>
+  <si>
+    <t>1. Cart page will be displayed
+2. Checkout: Your information page will be displayed
+3. Fill the First Name, Last Name, Zip/Postal Code fields
+4. Checkout: Overview will be displayed with Finish and Cancel buttons</t>
+  </si>
+  <si>
+    <t>TC304</t>
+  </si>
+  <si>
+    <t>Verify that user clicks on Cancelling the order from Checkout page</t>
+  </si>
+  <si>
+    <t>1. Enter the user information
+2. Click on Continue button
+3. Click on Cancel button</t>
+  </si>
+  <si>
+    <t>1. Fill the First Name, Last Name, Zip/Postal Code fields
+2. Checkout: Overview will be displayed
+3. Return to Home page and product in the cart should not be removed.</t>
   </si>
 </sst>
 </file>
@@ -542,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E170E6F-F863-48FA-9C66-E00A95112356}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,19 +907,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E900F11B-BF82-4A04-B629-E0FCDD75751C}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.21875" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="57.6640625" customWidth="1"/>
+    <col min="3" max="3" width="36.5546875" customWidth="1"/>
+    <col min="4" max="4" width="50.88671875" customWidth="1"/>
+    <col min="5" max="5" width="37.44140625" customWidth="1"/>
     <col min="6" max="6" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -741,26 +946,225 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD38535-BC53-4B07-B5C3-2B1F90AFB411}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="62.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="35.5546875" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A0CD8D-320D-4A2F-8462-23ABD865AE51}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.109375" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="30.21875" customWidth="1"/>
+    <col min="2" max="2" width="59" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.21875" customWidth="1"/>
+    <col min="5" max="5" width="45.33203125" customWidth="1"/>
     <col min="6" max="6" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -787,96 +1191,72 @@
         <v>7</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD38535-BC53-4B07-B5C3-2B1F90AFB411}">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="26.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F22DC05C-9456-4B64-B9D4-DED0707E7485}">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="23.109375" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="30.21875" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
+    <row r="2" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>